<commit_message>
some UI changes and new user role to incorporate demo for gastro
</commit_message>
<xml_diff>
--- a/Schablonen/Radiolearn.xlsx
+++ b/Schablonen/Radiolearn.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\radiospeech\Schablonen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ED8B5B-5064-4C35-9CE5-90AC7650E7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="41180" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" iterate="1" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -964,9 +973,6 @@
     <t>ZahlBruch</t>
   </si>
   <si>
-    <t>beträgt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Die Herz-Thorax-Relation beträgt %H1%. </t>
   </si>
   <si>
@@ -1441,9 +1447,6 @@
     <t>W8</t>
   </si>
   <si>
-    <t xml:space="preserve">Lokalisation: </t>
-  </si>
-  <si>
     <t>Verkalkung [lokalisiert in %W8%]</t>
   </si>
   <si>
@@ -1519,9 +1522,6 @@
     <t>S9</t>
   </si>
   <si>
-    <t>auf Höhe …</t>
-  </si>
-  <si>
     <t>Osteochondrose</t>
   </si>
   <si>
@@ -1643,37 +1643,47 @@
   </si>
   <si>
     <t>im ...</t>
+  </si>
+  <si>
+    <t>auf Höhe ...</t>
+  </si>
+  <si>
+    <t>Lokalisation: ...</t>
+  </si>
+  <si>
+    <t>beträgt ...</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -1683,7 +1693,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1693,46 +1703,54 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1922,37 +1940,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M99" sqref="M99"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.43"/>
-    <col customWidth="1" min="2" max="2" width="8.29"/>
-    <col customWidth="1" min="3" max="3" width="32.0"/>
-    <col customWidth="1" min="4" max="4" width="115.71"/>
-    <col customWidth="1" min="5" max="6" width="7.0"/>
-    <col customWidth="1" min="7" max="7" width="15.86"/>
-    <col customWidth="1" min="8" max="8" width="12.57"/>
-    <col customWidth="1" min="9" max="9" width="72.71"/>
-    <col customWidth="1" min="10" max="10" width="10.14"/>
-    <col customWidth="1" min="11" max="11" width="40.57"/>
-    <col customWidth="1" min="12" max="12" width="68.14"/>
-    <col customWidth="1" min="13" max="13" width="26.57"/>
-    <col customWidth="1" min="14" max="14" width="170.86"/>
-    <col customWidth="1" min="15" max="15" width="81.14"/>
-    <col customWidth="1" min="16" max="26" width="8.71"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="115.7265625" customWidth="1"/>
+    <col min="5" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="9" max="9" width="72.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.08984375" customWidth="1"/>
+    <col min="11" max="11" width="40.54296875" customWidth="1"/>
+    <col min="12" max="12" width="68.08984375" customWidth="1"/>
+    <col min="13" max="13" width="26.54296875" customWidth="1"/>
+    <col min="14" max="14" width="170.81640625" customWidth="1"/>
+    <col min="15" max="15" width="81.08984375" customWidth="1"/>
+    <col min="16" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1999,7 +2019,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2019,7 +2039,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
@@ -2033,7 +2053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2047,7 +2067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2067,7 +2087,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
@@ -2078,7 +2098,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -2086,7 +2106,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2109,7 +2129,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
@@ -2135,7 +2155,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J10" s="1" t="s">
         <v>47</v>
       </c>
@@ -2146,7 +2166,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2157,7 +2177,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>53</v>
       </c>
@@ -2183,7 +2203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J13" s="1" t="s">
         <v>57</v>
       </c>
@@ -2194,7 +2214,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2205,7 +2225,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>59</v>
       </c>
@@ -2231,7 +2251,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2242,7 +2262,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J17" s="1" t="s">
         <v>64</v>
       </c>
@@ -2253,7 +2273,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
         <v>65</v>
       </c>
@@ -2279,7 +2299,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J19" s="1" t="s">
         <v>69</v>
       </c>
@@ -2290,7 +2310,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J20" s="1" t="s">
         <v>70</v>
       </c>
@@ -2301,7 +2321,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
         <v>71</v>
       </c>
@@ -2327,7 +2347,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J22" s="1" t="s">
         <v>74</v>
       </c>
@@ -2338,7 +2358,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
@@ -2364,7 +2384,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J24" s="1" t="s">
         <v>79</v>
       </c>
@@ -2375,7 +2395,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="1" t="s">
         <v>80</v>
       </c>
@@ -2401,7 +2421,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J26" s="1" t="s">
         <v>84</v>
       </c>
@@ -2412,7 +2432,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
         <v>85</v>
       </c>
@@ -2438,7 +2458,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J28" s="1" t="s">
         <v>89</v>
       </c>
@@ -2449,7 +2469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
         <v>90</v>
       </c>
@@ -2472,7 +2492,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
         <v>94</v>
       </c>
@@ -2495,7 +2515,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C31" s="1" t="s">
         <v>97</v>
       </c>
@@ -2518,7 +2538,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="1" t="s">
         <v>101</v>
       </c>
@@ -2541,7 +2561,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J33" s="1" t="s">
         <v>105</v>
       </c>
@@ -2552,7 +2572,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C34" s="1" t="s">
         <v>108</v>
       </c>
@@ -2578,7 +2598,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J35" s="1" t="s">
         <v>111</v>
       </c>
@@ -2589,7 +2609,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J36" s="1" t="s">
         <v>114</v>
       </c>
@@ -2600,7 +2620,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
+    <row r="37" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="1" t="s">
         <v>117</v>
       </c>
@@ -2623,7 +2643,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="J38" s="1" t="s">
@@ -2639,7 +2659,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="J39" s="1" t="s">
@@ -2655,7 +2675,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J40" s="1" t="s">
         <v>128</v>
       </c>
@@ -2666,7 +2686,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
+    <row r="41" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C41" s="1" t="s">
         <v>131</v>
       </c>
@@ -2689,7 +2709,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
+    <row r="42" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C42" s="1" t="s">
         <v>135</v>
       </c>
@@ -2715,7 +2735,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
+    <row r="43" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C43" s="1" t="s">
         <v>142</v>
       </c>
@@ -2738,7 +2758,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" ht="14.25" customHeight="1">
+    <row r="44" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C44" s="1" t="s">
         <v>148</v>
       </c>
@@ -2752,7 +2772,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" ht="14.25" customHeight="1">
+    <row r="45" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C45" s="1" t="s">
         <v>150</v>
       </c>
@@ -2775,7 +2795,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" ht="14.25" customHeight="1">
+    <row r="46" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J46" s="1" t="s">
         <v>154</v>
       </c>
@@ -2786,7 +2806,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" ht="14.25" customHeight="1">
+    <row r="47" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C47" s="1" t="s">
         <v>157</v>
       </c>
@@ -2809,7 +2829,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" ht="14.25" customHeight="1">
+    <row r="48" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C48" s="1" t="s">
         <v>161</v>
       </c>
@@ -2832,7 +2852,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="49" ht="14.25" customHeight="1">
+    <row r="49" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J49" s="1" t="s">
         <v>164</v>
       </c>
@@ -2843,7 +2863,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" ht="14.25" customHeight="1">
+    <row r="50" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C50" s="1" t="s">
         <v>165</v>
       </c>
@@ -2866,7 +2886,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
+    <row r="51" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J51" s="1" t="s">
         <v>171</v>
       </c>
@@ -2875,7 +2895,7 @@
       </c>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" ht="14.25" customHeight="1">
+    <row r="52" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>33</v>
       </c>
@@ -2883,7 +2903,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
+    <row r="53" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>174</v>
       </c>
@@ -2906,7 +2926,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="54" ht="14.25" customHeight="1">
+    <row r="54" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C54" s="1" t="s">
         <v>179</v>
       </c>
@@ -2932,7 +2952,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="55" ht="14.25" customHeight="1">
+    <row r="55" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J55" s="1" t="s">
         <v>186</v>
       </c>
@@ -2944,7 +2964,7 @@
       </c>
       <c r="N55" s="6"/>
     </row>
-    <row r="56" ht="14.25" customHeight="1">
+    <row r="56" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C56" s="1" t="s">
         <v>189</v>
       </c>
@@ -2970,7 +2990,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" ht="14.25" customHeight="1">
+    <row r="57" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J57" s="1" t="s">
         <v>194</v>
       </c>
@@ -2982,7 +3002,7 @@
       </c>
       <c r="N57" s="6"/>
     </row>
-    <row r="58" ht="14.25" customHeight="1">
+    <row r="58" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C58" s="1" t="s">
         <v>195</v>
       </c>
@@ -3008,7 +3028,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="59" ht="14.25" customHeight="1">
+    <row r="59" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J59" s="1" t="s">
         <v>200</v>
       </c>
@@ -3020,7 +3040,7 @@
       </c>
       <c r="N59" s="6"/>
     </row>
-    <row r="60" ht="14.25" customHeight="1">
+    <row r="60" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>33</v>
       </c>
@@ -3028,7 +3048,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" ht="14.25" customHeight="1">
+    <row r="61" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>202</v>
       </c>
@@ -3054,7 +3074,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" ht="14.25" customHeight="1">
+    <row r="62" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C62" s="1" t="s">
         <v>208</v>
       </c>
@@ -3080,7 +3100,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" ht="14.25" customHeight="1">
+    <row r="63" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J63" s="1" t="s">
         <v>212</v>
       </c>
@@ -3091,7 +3111,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="64" ht="14.25" customHeight="1">
+    <row r="64" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J64" s="1" t="s">
         <v>214</v>
       </c>
@@ -3102,7 +3122,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" ht="14.25" customHeight="1">
+    <row r="65" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J65" s="1" t="s">
         <v>217</v>
       </c>
@@ -3113,7 +3133,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
+    <row r="66" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C66" s="1" t="s">
         <v>219</v>
       </c>
@@ -3139,7 +3159,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="67" ht="14.25" customHeight="1">
+    <row r="67" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J67" s="1" t="s">
         <v>223</v>
       </c>
@@ -3150,7 +3170,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
+    <row r="68" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J68" s="1" t="s">
         <v>224</v>
       </c>
@@ -3161,7 +3181,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" ht="14.25" customHeight="1">
+    <row r="69" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J69" s="1" t="s">
         <v>225</v>
       </c>
@@ -3175,7 +3195,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
+    <row r="70" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C70" s="1" t="s">
         <v>229</v>
       </c>
@@ -3201,7 +3221,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" ht="14.25" customHeight="1">
+    <row r="71" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J71" s="1" t="s">
         <v>233</v>
       </c>
@@ -3212,7 +3232,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
+    <row r="72" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J72" s="1" t="s">
         <v>234</v>
       </c>
@@ -3223,7 +3243,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="73" ht="14.25" customHeight="1">
+    <row r="73" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J73" s="1" t="s">
         <v>235</v>
       </c>
@@ -3237,7 +3257,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="74" ht="14.25" customHeight="1">
+    <row r="74" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C74" s="1" t="s">
         <v>236</v>
       </c>
@@ -3260,7 +3280,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="75" ht="14.25" customHeight="1">
+    <row r="75" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J75" s="1" t="s">
         <v>239</v>
       </c>
@@ -3271,7 +3291,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="76" ht="14.25" customHeight="1">
+    <row r="76" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C76" s="1" t="s">
         <v>242</v>
       </c>
@@ -3294,7 +3314,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="77" ht="14.25" customHeight="1">
+    <row r="77" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J77" s="1" t="s">
         <v>246</v>
       </c>
@@ -3305,7 +3325,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="78" ht="14.25" customHeight="1">
+    <row r="78" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C78" s="1" t="s">
         <v>247</v>
       </c>
@@ -3328,7 +3348,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" ht="14.25" customHeight="1">
+    <row r="79" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J79" s="1" t="s">
         <v>250</v>
       </c>
@@ -3339,7 +3359,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="80" ht="14.25" customHeight="1">
+    <row r="80" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C80" s="1" t="s">
         <v>251</v>
       </c>
@@ -3359,7 +3379,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" ht="14.25" customHeight="1">
+    <row r="81" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J81" s="1" t="s">
         <v>254</v>
       </c>
@@ -3370,7 +3390,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="82" ht="14.25" customHeight="1">
+    <row r="82" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J82" s="1" t="s">
         <v>255</v>
       </c>
@@ -3381,7 +3401,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
+    <row r="83" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C83" s="1" t="s">
         <v>256</v>
       </c>
@@ -3401,7 +3421,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" ht="14.25" customHeight="1">
+    <row r="84" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>33</v>
       </c>
@@ -3409,7 +3429,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" ht="14.25" customHeight="1">
+    <row r="85" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>261</v>
       </c>
@@ -3429,7 +3449,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="86" ht="14.25" customHeight="1">
+    <row r="86" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C86" s="1" t="s">
         <v>264</v>
       </c>
@@ -3455,7 +3475,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="87" ht="14.25" customHeight="1">
+    <row r="87" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C87" s="1" t="s">
         <v>269</v>
       </c>
@@ -3484,7 +3504,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="88" ht="14.25" customHeight="1">
+    <row r="88" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>277</v>
       </c>
@@ -3495,7 +3515,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="89" ht="14.25" customHeight="1">
+    <row r="89" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>280</v>
       </c>
@@ -3515,7 +3535,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="90" ht="14.25" customHeight="1">
+    <row r="90" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C90" s="1" t="s">
         <v>284</v>
       </c>
@@ -3532,7 +3552,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="91" ht="14.25" customHeight="1">
+    <row r="91" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C91" s="1" t="s">
         <v>287</v>
       </c>
@@ -3549,7 +3569,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="92" ht="14.25" customHeight="1">
+    <row r="92" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C92" s="1" t="s">
         <v>290</v>
       </c>
@@ -3581,7 +3601,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="93" ht="14.25" customHeight="1">
+    <row r="93" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J93" s="1" t="s">
         <v>298</v>
       </c>
@@ -3592,7 +3612,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="94" ht="14.25" customHeight="1">
+    <row r="94" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>300</v>
       </c>
@@ -3612,7 +3632,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="95" ht="14.25" customHeight="1">
+    <row r="95" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C95" s="1" t="s">
         <v>269</v>
       </c>
@@ -3629,7 +3649,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="96" ht="14.25" customHeight="1">
+    <row r="96" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C96" s="1" t="s">
         <v>307</v>
       </c>
@@ -3643,7 +3663,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="97" ht="14.25" customHeight="1">
+    <row r="97" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C97" s="1" t="s">
         <v>310</v>
       </c>
@@ -3657,7 +3677,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="98" ht="14.25" customHeight="1">
+    <row r="98" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C98" s="1" t="s">
         <v>313</v>
       </c>
@@ -3671,38 +3691,38 @@
         <v>316</v>
       </c>
       <c r="M98" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="N98" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="N98" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="99" ht="14.25" customHeight="1">
+    </row>
+    <row r="99" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N99" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G100" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="J100" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="K100" s="1" t="s">
         <v>43</v>
@@ -3711,21 +3731,21 @@
         <v>213</v>
       </c>
       <c r="N100" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C101" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="101" ht="14.25" customHeight="1">
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="G101" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="J101" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="J101" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>43</v>
@@ -3734,21 +3754,21 @@
         <v>213</v>
       </c>
       <c r="N101" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C102" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="102" ht="14.25" customHeight="1">
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="G102" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="J102" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="J102" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>43</v>
@@ -3757,21 +3777,21 @@
         <v>213</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="103" ht="14.25" customHeight="1">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C103" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D103" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="J103" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="J103" s="1" t="s">
-        <v>334</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>43</v>
@@ -3780,92 +3800,92 @@
         <v>213</v>
       </c>
       <c r="N103" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G104" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="N104" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="N104" s="1" t="s">
+      <c r="O104" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="O104" s="1" t="s">
+    </row>
+    <row r="105" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C105" s="1" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="105" ht="14.25" customHeight="1">
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="G105" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="N105" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="G105" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="N105" s="1" t="s">
+      <c r="O105" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="O105" s="1" t="s">
+    </row>
+    <row r="106" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C106" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="106" ht="14.25" customHeight="1">
-      <c r="C106" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="G106" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="N106" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="G106" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="N106" s="1" t="s">
+      <c r="O106" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="O106" s="1" t="s">
+    </row>
+    <row r="107" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C107" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="107" ht="14.25" customHeight="1">
-      <c r="C107" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="G107" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="N107" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="G107" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="N107" s="1" t="s">
+      <c r="O107" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="O107" s="1" t="s">
+    </row>
+    <row r="108" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C108" s="1" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="108" ht="14.25" customHeight="1">
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="J108" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="J108" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="K108" s="2" t="s">
         <v>187</v>
@@ -3874,52 +3894,52 @@
         <v>188</v>
       </c>
     </row>
-    <row r="109" ht="14.25" customHeight="1">
+    <row r="109" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N109" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G110" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="N110" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="N110" s="1" t="s">
+      <c r="O110" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="O110" s="1" t="s">
+    </row>
+    <row r="111" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C111" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="111" ht="14.25" customHeight="1">
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="J111" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="J111" s="1" t="s">
-        <v>364</v>
       </c>
       <c r="K111" s="2" t="s">
         <v>187</v>
@@ -3928,15 +3948,15 @@
         <v>188</v>
       </c>
       <c r="N111" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="O111" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="O111" s="1" t="s">
+    </row>
+    <row r="112" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J112" s="1" t="s">
         <v>366</v>
-      </c>
-    </row>
-    <row r="112" ht="14.25" customHeight="1">
-      <c r="J112" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="K112" s="1" t="s">
         <v>43</v>
@@ -3945,57 +3965,57 @@
         <v>213</v>
       </c>
     </row>
-    <row r="113" ht="14.25" customHeight="1">
+    <row r="113" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J113" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="K113" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="K113" s="1" t="s">
+      <c r="L113" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="L113" s="1" t="s">
+    </row>
+    <row r="114" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J114" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="114" ht="14.25" customHeight="1">
-      <c r="J114" s="1" t="s">
+      <c r="K114" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="K114" s="1" t="s">
+      <c r="L114" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="L114" s="1" t="s">
+    </row>
+    <row r="115" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C115" s="1" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="115" ht="14.25" customHeight="1">
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="G115" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="N115" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="N115" s="1" t="s">
+      <c r="O115" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="O115" s="1" t="s">
+    </row>
+    <row r="116" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C116" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="116" ht="14.25" customHeight="1">
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="G116" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="J116" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="J116" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="K116" s="2" t="s">
         <v>187</v>
@@ -4004,15 +4024,15 @@
         <v>188</v>
       </c>
       <c r="N116" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="O116" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="O116" s="1" t="s">
+    </row>
+    <row r="117" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J117" s="1" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="117" ht="14.25" customHeight="1">
-      <c r="J117" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>43</v>
@@ -4021,76 +4041,76 @@
         <v>213</v>
       </c>
     </row>
-    <row r="118" ht="14.25" customHeight="1">
+    <row r="118" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J118" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K118" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="K118" s="1" t="s">
+      <c r="M118" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="M118" s="1" t="s">
+    </row>
+    <row r="119" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J119" s="1" t="s">
         <v>387</v>
-      </c>
-    </row>
-    <row r="119" ht="14.25" customHeight="1">
-      <c r="J119" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>106</v>
       </c>
       <c r="M119" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="120" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J120" s="1" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="120" ht="14.25" customHeight="1">
-      <c r="J120" s="1" t="s">
+      <c r="K120" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M120" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="K120" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M120" s="1" t="s">
+    </row>
+    <row r="121" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J121" s="1" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="121" ht="14.25" customHeight="1">
-      <c r="J121" s="1" t="s">
+      <c r="K121" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M121" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="K121" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M121" s="1" t="s">
+    </row>
+    <row r="122" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C122" s="1" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="122" ht="14.25" customHeight="1">
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="N122" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="123" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C123" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G123" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="G122" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="N122" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="123" ht="14.25" customHeight="1">
-      <c r="C123" s="1" t="s">
+      <c r="J123" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="J123" s="1" t="s">
-        <v>398</v>
       </c>
       <c r="K123" s="2" t="s">
         <v>187</v>
@@ -4099,12 +4119,12 @@
         <v>188</v>
       </c>
       <c r="N123" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="124" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J124" s="1" t="s">
         <v>399</v>
-      </c>
-    </row>
-    <row r="124" ht="14.25" customHeight="1">
-      <c r="J124" s="1" t="s">
-        <v>400</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>43</v>
@@ -4113,59 +4133,59 @@
         <v>213</v>
       </c>
     </row>
-    <row r="125" ht="14.25" customHeight="1">
+    <row r="125" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J125" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="K125" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="K125" s="1" t="s">
+      <c r="L125" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="L125" s="1" t="s">
+    </row>
+    <row r="126" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J126" s="1" t="s">
         <v>403</v>
-      </c>
-    </row>
-    <row r="126" ht="14.25" customHeight="1">
-      <c r="J126" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>106</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="127" ht="14.25" customHeight="1">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="127" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J127" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="K127" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="K127" s="1" t="s">
+      <c r="L127" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="128" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C128" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="L127" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="128" ht="14.25" customHeight="1">
-      <c r="C128" s="1" t="s">
+      <c r="N128" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="N128" s="1" t="s">
+    </row>
+    <row r="129" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C129" s="1" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="129" ht="14.25" customHeight="1">
-      <c r="C129" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="J129" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="J129" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="K129" s="2" t="s">
         <v>187</v>
@@ -4174,26 +4194,26 @@
         <v>188</v>
       </c>
       <c r="N129" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="O129" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="O129" s="1" t="s">
+    </row>
+    <row r="130" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J130" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="130" ht="14.25" customHeight="1">
-      <c r="J130" s="1" t="s">
+      <c r="K130" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="K130" s="1" t="s">
+      <c r="L130" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="L130" s="1" t="s">
+    </row>
+    <row r="131" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J131" s="1" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="131" ht="14.25" customHeight="1">
-      <c r="J131" s="1" t="s">
-        <v>417</v>
       </c>
       <c r="K131" s="1" t="s">
         <v>43</v>
@@ -4202,26 +4222,26 @@
         <v>213</v>
       </c>
     </row>
-    <row r="132" ht="14.25" customHeight="1">
+    <row r="132" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J132" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="L132" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C133" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="K132" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="L132" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="133" ht="14.25" customHeight="1">
-      <c r="C133" s="1" t="s">
+      <c r="D133" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="J133" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="J133" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="K133" s="2" t="s">
         <v>187</v>
@@ -4230,15 +4250,15 @@
         <v>188</v>
       </c>
       <c r="N133" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="O133" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="O133" s="1" t="s">
+    </row>
+    <row r="134" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J134" s="1" t="s">
         <v>422</v>
-      </c>
-    </row>
-    <row r="134" ht="14.25" customHeight="1">
-      <c r="J134" s="1" t="s">
-        <v>423</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>43</v>
@@ -4247,26 +4267,26 @@
         <v>213</v>
       </c>
     </row>
-    <row r="135" ht="14.25" customHeight="1">
+    <row r="135" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J135" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="K135" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="K135" s="1" t="s">
+      <c r="L135" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="L135" s="1" t="s">
+    </row>
+    <row r="136" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C136" s="1" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="136" ht="14.25" customHeight="1">
-      <c r="C136" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="J136" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="J136" s="1" t="s">
-        <v>429</v>
       </c>
       <c r="K136" s="2" t="s">
         <v>187</v>
@@ -4275,15 +4295,15 @@
         <v>188</v>
       </c>
       <c r="N136" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="O136" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="O136" s="1" t="s">
+    </row>
+    <row r="137" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J137" s="1" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="137" ht="14.25" customHeight="1">
-      <c r="J137" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="K137" s="1" t="s">
         <v>43</v>
@@ -4292,26 +4312,26 @@
         <v>213</v>
       </c>
     </row>
-    <row r="138" ht="14.25" customHeight="1">
+    <row r="138" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J138" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C139" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="K138" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="L138" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="139" ht="14.25" customHeight="1">
-      <c r="C139" s="1" t="s">
+      <c r="D139" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="J139" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="J139" s="1" t="s">
-        <v>435</v>
       </c>
       <c r="K139" s="2" t="s">
         <v>187</v>
@@ -4320,15 +4340,15 @@
         <v>188</v>
       </c>
       <c r="N139" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="O139" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="O139" s="1" t="s">
+    </row>
+    <row r="140" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J140" s="1" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="140" ht="14.25" customHeight="1">
-      <c r="J140" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="K140" s="1" t="s">
         <v>43</v>
@@ -4337,45 +4357,45 @@
         <v>213</v>
       </c>
     </row>
-    <row r="141" ht="14.25" customHeight="1">
+    <row r="141" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J141" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C142" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="K141" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="L141" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="142" ht="14.25" customHeight="1">
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="N142" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="N142" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="143" ht="14.25" customHeight="1">
+    </row>
+    <row r="143" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N143" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="1" t="s">
-        <v>443</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>16</v>
@@ -4384,21 +4404,21 @@
         <v>38</v>
       </c>
       <c r="N144" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C145" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="145" ht="14.25" customHeight="1">
-      <c r="C145" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="D145" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K145" s="1" t="s">
         <v>43</v>
@@ -4407,94 +4427,94 @@
         <v>213</v>
       </c>
       <c r="N145" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C146" s="1" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="146" ht="14.25" customHeight="1">
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>450</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N146" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C147" s="1" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="147" ht="14.25" customHeight="1">
-      <c r="C147" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="D147" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N147" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C148" s="1" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="148" ht="14.25" customHeight="1">
-      <c r="C148" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="D148" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N148" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C149" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="149" ht="14.25" customHeight="1">
-      <c r="C149" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="D149" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N149" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="O149" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="O149" s="1" t="s">
+    </row>
+    <row r="150" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C150" s="1" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="150" ht="14.25" customHeight="1">
-      <c r="C150" s="1" t="s">
-        <v>459</v>
-      </c>
       <c r="D150" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N150" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C151" s="1" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="151" ht="14.25" customHeight="1">
-      <c r="C151" s="1" t="s">
+      <c r="D151" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K151" s="1" t="s">
         <v>43</v>
@@ -4503,29 +4523,29 @@
         <v>213</v>
       </c>
       <c r="N151" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O151" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="O151" s="1" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="152" ht="14.25" customHeight="1">
+    </row>
+    <row r="152" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N152" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="1" t="s">
+      <c r="C153" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="D153" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>16</v>
@@ -4534,21 +4554,21 @@
         <v>38</v>
       </c>
       <c r="N153" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C154" s="1" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="154" ht="14.25" customHeight="1">
-      <c r="C154" s="1" t="s">
+      <c r="D154" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="J154" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="I154" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="J154" s="1" t="s">
-        <v>472</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>43</v>
@@ -4557,44 +4577,44 @@
         <v>213</v>
       </c>
       <c r="N154" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C155" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="155" ht="14.25" customHeight="1">
-      <c r="C155" s="1" t="s">
+      <c r="D155" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="J155" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="I155" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="J155" s="1" t="s">
+      <c r="K155" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="N155" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="K155" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M155" s="1" t="s">
+    </row>
+    <row r="156" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C156" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="N155" s="1" t="s">
+      <c r="D156" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="156" ht="14.25" customHeight="1">
-      <c r="C156" s="1" t="s">
+      <c r="I156" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="J156" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="I156" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="J156" s="1" t="s">
-        <v>480</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>43</v>
@@ -4603,26 +4623,26 @@
         <v>213</v>
       </c>
       <c r="N156" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="O156" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J157" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="K157" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="O156" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="157" ht="14.25" customHeight="1">
-      <c r="J157" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="K157" s="1" t="s">
-        <v>483</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="158" ht="14.25" customHeight="1">
+    <row r="158" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J158" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K158" s="1" t="s">
         <v>187</v>
@@ -4631,18 +4651,18 @@
         <v>188</v>
       </c>
     </row>
-    <row r="159" ht="14.25" customHeight="1">
+    <row r="159" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C159" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="I159" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="J159" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="I159" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="J159" s="1" t="s">
-        <v>487</v>
       </c>
       <c r="K159" s="1" t="s">
         <v>43</v>
@@ -4651,26 +4671,26 @@
         <v>213</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="160" ht="14.25" customHeight="1">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J160" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="161" ht="14.25" customHeight="1">
+    <row r="161" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J161" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K161" s="1" t="s">
         <v>187</v>
@@ -4679,37 +4699,37 @@
         <v>188</v>
       </c>
     </row>
-    <row r="162" ht="14.25" customHeight="1">
+    <row r="162" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>33</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="163" ht="14.25" customHeight="1">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>277</v>
       </c>
       <c r="H163" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="N163" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="N163" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="164" ht="14.25" customHeight="1">
-      <c r="A164" s="1" t="s">
-        <v>494</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>16</v>
@@ -4718,175 +4738,175 @@
         <v>38</v>
       </c>
       <c r="N164" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C165" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I165" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J165" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="165" ht="14.25" customHeight="1">
-      <c r="C165" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="H165" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I165" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J165" s="1" t="s">
-        <v>499</v>
-      </c>
       <c r="K165" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L165" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N165" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J166" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M166" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C167" s="1" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="166" ht="14.25" customHeight="1">
-      <c r="J166" s="1" t="s">
+      <c r="D167" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J167" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="K166" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M166" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="167" ht="14.25" customHeight="1">
-      <c r="C167" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="H167" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I167" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J167" s="1" t="s">
-        <v>504</v>
-      </c>
       <c r="K167" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L167" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N167" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J168" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K168" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M168" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C169" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="N169" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C170" s="1" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="168" ht="14.25" customHeight="1">
-      <c r="J168" s="1" t="s">
+      <c r="D170" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J170" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="K168" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M168" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="169" ht="14.25" customHeight="1">
-      <c r="C169" s="1" t="s">
+      <c r="K170" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="L170" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="H169" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I169" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="N169" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="170" ht="14.25" customHeight="1">
-      <c r="C170" s="1" t="s">
+      <c r="N170" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="D170" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="I170" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J170" s="1" t="s">
+    </row>
+    <row r="171" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J171" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="K170" s="1" t="s">
+      <c r="K171" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M171" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C172" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="L170" s="1" t="s">
+      <c r="D172" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="N170" s="1" t="s">
+      <c r="H172" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J172" s="1" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="171" ht="14.25" customHeight="1">
-      <c r="J171" s="1" t="s">
+      <c r="K172" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="K171" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M171" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="172" ht="14.25" customHeight="1">
-      <c r="C172" s="1" t="s">
+      <c r="L172" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="D172" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="H172" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I172" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J172" s="1" t="s">
+      <c r="N172" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="K172" s="1" t="s">
+    </row>
+    <row r="173" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C173" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="L172" s="1" t="s">
+      <c r="D173" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I173" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J173" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="N172" s="1" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="173" ht="14.25" customHeight="1">
-      <c r="C173" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="H173" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I173" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J173" s="1" t="s">
-        <v>519</v>
       </c>
       <c r="K173" s="1" t="s">
         <v>43</v>
@@ -4895,64 +4915,64 @@
         <v>213</v>
       </c>
       <c r="N173" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C174" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I174" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C175" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D175" s="1" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="174" ht="14.25" customHeight="1">
-      <c r="C174" s="1" t="s">
+      <c r="H175" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J175" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="D174" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="H174" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I174" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="175" ht="14.25" customHeight="1">
-      <c r="C175" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="H175" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I175" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J175" s="1" t="s">
-        <v>524</v>
-      </c>
       <c r="K175" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L175" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N175" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C176" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J176" s="1" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row r="176" ht="14.25" customHeight="1">
-      <c r="C176" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="H176" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="I176" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J176" s="1" t="s">
-        <v>528</v>
       </c>
       <c r="K176" s="1" t="s">
         <v>43</v>
@@ -4961,35 +4981,35 @@
         <v>213</v>
       </c>
       <c r="N176" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="177" ht="14.25" customHeight="1">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="177" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J177" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="K177" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L177" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="178" ht="14.25" customHeight="1">
+    <row r="178" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C178" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H178" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="K178" s="1" t="s">
         <v>43</v>
@@ -4998,883 +5018,881 @@
         <v>213</v>
       </c>
       <c r="N178" s="1" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="179" ht="14.25" customHeight="1">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="179" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J179" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="K179" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L179" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="180" ht="14.25" customHeight="1">
+    <row r="180" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C180" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J180" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="K180" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="L180" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="D180" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="I180" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="J180" s="1" t="s">
+      <c r="M180" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="K180" s="1" t="s">
+      <c r="N180" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="L180" s="1" t="s">
+      <c r="O180" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="M180" s="1" t="s">
+    </row>
+    <row r="181" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J181" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="N180" s="1" t="s">
+      <c r="K181" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M181" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="O180" s="1" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="181" ht="14.25" customHeight="1">
-      <c r="J181" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="K181" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M181" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="182" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="187" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="188" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="189" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="190" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="191" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="192" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added ellipsis replacement in backend and fixed MC variable parsing
</commit_message>
<xml_diff>
--- a/Schablonen/Radiolearn.xlsx
+++ b/Schablonen/Radiolearn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\radiospeech\Schablonen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ED8B5B-5064-4C35-9CE5-90AC7650E7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35FED3B-AB91-4F9A-98C8-0A5FDD934BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="41180" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="546">
   <si>
     <t>Gliederung</t>
   </si>
@@ -1652,6 +1652,12 @@
   </si>
   <si>
     <t>beträgt ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">am ehesten Mamillenschatten; </t>
+  </si>
+  <si>
+    <t>Ausdehnung über … cm</t>
   </si>
 </sst>
 </file>
@@ -1734,7 +1740,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1949,30 +1955,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M99" sqref="M99"/>
+    <sheetView tabSelected="1" topLeftCell="G106" workbookViewId="0">
+      <selection activeCell="M126" sqref="M126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="115.7265625" customWidth="1"/>
+    <col min="4" max="4" width="115.7109375" customWidth="1"/>
     <col min="5" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" customWidth="1"/>
-    <col min="9" max="9" width="72.7265625" customWidth="1"/>
-    <col min="10" max="10" width="10.08984375" customWidth="1"/>
-    <col min="11" max="11" width="40.54296875" customWidth="1"/>
-    <col min="12" max="12" width="68.08984375" customWidth="1"/>
-    <col min="13" max="13" width="26.54296875" customWidth="1"/>
-    <col min="14" max="14" width="170.81640625" customWidth="1"/>
-    <col min="15" max="15" width="81.08984375" customWidth="1"/>
-    <col min="16" max="26" width="8.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="72.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" customWidth="1"/>
+    <col min="12" max="12" width="68.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" customWidth="1"/>
+    <col min="14" max="14" width="170.85546875" customWidth="1"/>
+    <col min="15" max="15" width="81.140625" customWidth="1"/>
+    <col min="16" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2067,7 +2073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2087,7 +2093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J10" s="1" t="s">
         <v>47</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>53</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J13" s="1" t="s">
         <v>57</v>
       </c>
@@ -2214,7 +2220,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>59</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J17" s="1" t="s">
         <v>64</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>65</v>
       </c>
@@ -2299,7 +2305,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J19" s="1" t="s">
         <v>69</v>
       </c>
@@ -2310,7 +2316,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J20" s="1" t="s">
         <v>70</v>
       </c>
@@ -2321,7 +2327,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>71</v>
       </c>
@@ -2347,7 +2353,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J22" s="1" t="s">
         <v>74</v>
       </c>
@@ -2358,7 +2364,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
@@ -2384,7 +2390,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J24" s="1" t="s">
         <v>79</v>
       </c>
@@ -2395,7 +2401,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>80</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J26" s="1" t="s">
         <v>84</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>85</v>
       </c>
@@ -2458,7 +2464,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J28" s="1" t="s">
         <v>89</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>90</v>
       </c>
@@ -2492,7 +2498,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>94</v>
       </c>
@@ -2515,7 +2521,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>97</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>101</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J33" s="1" t="s">
         <v>105</v>
       </c>
@@ -2572,7 +2578,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>108</v>
       </c>
@@ -2598,7 +2604,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J35" s="1" t="s">
         <v>111</v>
       </c>
@@ -2609,7 +2615,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J36" s="1" t="s">
         <v>114</v>
       </c>
@@ -2620,7 +2626,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>117</v>
       </c>
@@ -2643,7 +2649,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="J38" s="1" t="s">
@@ -2659,7 +2665,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="J39" s="1" t="s">
@@ -2675,7 +2681,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J40" s="1" t="s">
         <v>128</v>
       </c>
@@ -2686,7 +2692,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>131</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>135</v>
       </c>
@@ -2735,7 +2741,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
         <v>142</v>
       </c>
@@ -2758,7 +2764,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>148</v>
       </c>
@@ -2772,7 +2778,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>150</v>
       </c>
@@ -2795,7 +2801,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J46" s="1" t="s">
         <v>154</v>
       </c>
@@ -2806,7 +2812,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>157</v>
       </c>
@@ -2829,7 +2835,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>161</v>
       </c>
@@ -2852,7 +2858,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J49" s="1" t="s">
         <v>164</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>165</v>
       </c>
@@ -2886,7 +2892,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J51" s="1" t="s">
         <v>171</v>
       </c>
@@ -2895,7 +2901,7 @@
       </c>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>33</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>174</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>179</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J55" s="1" t="s">
         <v>186</v>
       </c>
@@ -2964,7 +2970,7 @@
       </c>
       <c r="N55" s="6"/>
     </row>
-    <row r="56" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>189</v>
       </c>
@@ -2990,7 +2996,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J57" s="1" t="s">
         <v>194</v>
       </c>
@@ -3002,7 +3008,7 @@
       </c>
       <c r="N57" s="6"/>
     </row>
-    <row r="58" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>195</v>
       </c>
@@ -3028,7 +3034,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J59" s="1" t="s">
         <v>200</v>
       </c>
@@ -3040,7 +3046,7 @@
       </c>
       <c r="N59" s="6"/>
     </row>
-    <row r="60" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>33</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>202</v>
       </c>
@@ -3074,7 +3080,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="1" t="s">
         <v>208</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J63" s="1" t="s">
         <v>212</v>
       </c>
@@ -3111,7 +3117,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J64" s="1" t="s">
         <v>214</v>
       </c>
@@ -3122,7 +3128,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J65" s="1" t="s">
         <v>217</v>
       </c>
@@ -3133,7 +3139,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>219</v>
       </c>
@@ -3159,7 +3165,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="67" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J67" s="1" t="s">
         <v>223</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J68" s="1" t="s">
         <v>224</v>
       </c>
@@ -3181,7 +3187,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J69" s="1" t="s">
         <v>225</v>
       </c>
@@ -3195,7 +3201,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>229</v>
       </c>
@@ -3221,7 +3227,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J71" s="1" t="s">
         <v>233</v>
       </c>
@@ -3232,7 +3238,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J72" s="1" t="s">
         <v>234</v>
       </c>
@@ -3243,7 +3249,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="73" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J73" s="1" t="s">
         <v>235</v>
       </c>
@@ -3257,7 +3263,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="74" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
         <v>236</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="75" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J75" s="1" t="s">
         <v>239</v>
       </c>
@@ -3291,7 +3297,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="76" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1" t="s">
         <v>242</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="77" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J77" s="1" t="s">
         <v>246</v>
       </c>
@@ -3325,7 +3331,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="78" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="1" t="s">
         <v>247</v>
       </c>
@@ -3348,7 +3354,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J79" s="1" t="s">
         <v>250</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="80" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="1" t="s">
         <v>251</v>
       </c>
@@ -3379,7 +3385,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J81" s="1" t="s">
         <v>254</v>
       </c>
@@ -3390,7 +3396,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J82" s="1" t="s">
         <v>255</v>
       </c>
@@ -3401,7 +3407,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="1" t="s">
         <v>256</v>
       </c>
@@ -3421,7 +3427,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>33</v>
       </c>
@@ -3429,7 +3435,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>261</v>
       </c>
@@ -3449,7 +3455,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="1" t="s">
         <v>264</v>
       </c>
@@ -3475,7 +3481,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
         <v>269</v>
       </c>
@@ -3504,7 +3510,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>277</v>
       </c>
@@ -3515,7 +3521,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>280</v>
       </c>
@@ -3535,7 +3541,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
         <v>284</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
         <v>287</v>
       </c>
@@ -3569,7 +3575,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="1" t="s">
         <v>290</v>
       </c>
@@ -3601,7 +3607,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J93" s="1" t="s">
         <v>298</v>
       </c>
@@ -3612,7 +3618,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>300</v>
       </c>
@@ -3632,7 +3638,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="1" t="s">
         <v>269</v>
       </c>
@@ -3649,7 +3655,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="1" t="s">
         <v>307</v>
       </c>
@@ -3663,7 +3669,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="1" t="s">
         <v>310</v>
       </c>
@@ -3677,7 +3683,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C98" s="1" t="s">
         <v>313</v>
       </c>
@@ -3697,7 +3703,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>33</v>
       </c>
@@ -3705,7 +3711,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>319</v>
       </c>
@@ -3734,7 +3740,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C101" s="1" t="s">
         <v>324</v>
       </c>
@@ -3757,7 +3763,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C102" s="1" t="s">
         <v>328</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="1" t="s">
         <v>264</v>
       </c>
@@ -3803,7 +3809,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>335</v>
       </c>
@@ -3826,7 +3832,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C105" s="1" t="s">
         <v>341</v>
       </c>
@@ -3843,7 +3849,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C106" s="1" t="s">
         <v>345</v>
       </c>
@@ -3860,7 +3866,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C107" s="1" t="s">
         <v>349</v>
       </c>
@@ -3877,7 +3883,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
         <v>353</v>
       </c>
@@ -3894,7 +3900,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>33</v>
       </c>
@@ -3902,7 +3908,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>357</v>
       </c>
@@ -3928,7 +3934,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C111" s="1" t="s">
         <v>362</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J112" s="1" t="s">
         <v>366</v>
       </c>
@@ -3965,7 +3971,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="113" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J113" s="1" t="s">
         <v>367</v>
       </c>
@@ -3976,7 +3982,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="114" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J114" s="1" t="s">
         <v>370</v>
       </c>
@@ -3987,7 +3993,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="115" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C115" s="1" t="s">
         <v>373</v>
       </c>
@@ -4004,7 +4010,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="116" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="1" t="s">
         <v>378</v>
       </c>
@@ -4030,7 +4036,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="117" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J117" s="1" t="s">
         <v>383</v>
       </c>
@@ -4041,7 +4047,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="118" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J118" s="1" t="s">
         <v>384</v>
       </c>
@@ -4052,7 +4058,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="119" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J119" s="1" t="s">
         <v>387</v>
       </c>
@@ -4063,7 +4069,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="120" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J120" s="1" t="s">
         <v>389</v>
       </c>
@@ -4074,7 +4080,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J121" s="1" t="s">
         <v>391</v>
       </c>
@@ -4085,7 +4091,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="122" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C122" s="1" t="s">
         <v>393</v>
       </c>
@@ -4099,7 +4105,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="123" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C123" s="1" t="s">
         <v>396</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="124" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J124" s="1" t="s">
         <v>399</v>
       </c>
@@ -4133,7 +4139,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="125" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J125" s="1" t="s">
         <v>400</v>
       </c>
@@ -4144,7 +4150,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J126" s="1" t="s">
         <v>403</v>
       </c>
@@ -4152,10 +4158,10 @@
         <v>106</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="127" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="127" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J127" s="1" t="s">
         <v>404</v>
       </c>
@@ -4163,10 +4169,10 @@
         <v>405</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="128" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="128" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="1" t="s">
         <v>406</v>
       </c>
@@ -4177,7 +4183,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C129" s="1" t="s">
         <v>408</v>
       </c>
@@ -4200,7 +4206,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J130" s="1" t="s">
         <v>413</v>
       </c>
@@ -4211,7 +4217,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J131" s="1" t="s">
         <v>416</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J132" s="1" t="s">
         <v>417</v>
       </c>
@@ -4233,7 +4239,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C133" s="1" t="s">
         <v>418</v>
       </c>
@@ -4256,7 +4262,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J134" s="1" t="s">
         <v>422</v>
       </c>
@@ -4267,7 +4273,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J135" s="1" t="s">
         <v>423</v>
       </c>
@@ -4278,7 +4284,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C136" s="1" t="s">
         <v>426</v>
       </c>
@@ -4301,7 +4307,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J137" s="1" t="s">
         <v>431</v>
       </c>
@@ -4312,7 +4318,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J138" s="1" t="s">
         <v>432</v>
       </c>
@@ -4323,7 +4329,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C139" s="1" t="s">
         <v>433</v>
       </c>
@@ -4346,7 +4352,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J140" s="1" t="s">
         <v>437</v>
       </c>
@@ -4357,7 +4363,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J141" s="1" t="s">
         <v>438</v>
       </c>
@@ -4368,7 +4374,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C142" s="1" t="s">
         <v>439</v>
       </c>
@@ -4379,7 +4385,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>33</v>
       </c>
@@ -4387,7 +4393,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>442</v>
       </c>
@@ -4407,7 +4413,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C145" s="1" t="s">
         <v>445</v>
       </c>
@@ -4430,7 +4436,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C146" s="1" t="s">
         <v>448</v>
       </c>
@@ -4444,7 +4450,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C147" s="1" t="s">
         <v>451</v>
       </c>
@@ -4458,7 +4464,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C148" s="1" t="s">
         <v>453</v>
       </c>
@@ -4472,7 +4478,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C149" s="1" t="s">
         <v>455</v>
       </c>
@@ -4489,7 +4495,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C150" s="1" t="s">
         <v>458</v>
       </c>
@@ -4503,7 +4509,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
         <v>460</v>
       </c>
@@ -4529,7 +4535,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>33</v>
       </c>
@@ -4537,7 +4543,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>466</v>
       </c>
@@ -4557,7 +4563,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C154" s="1" t="s">
         <v>470</v>
       </c>
@@ -4580,7 +4586,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
         <v>473</v>
       </c>
@@ -4603,7 +4609,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C156" s="1" t="s">
         <v>476</v>
       </c>
@@ -4629,7 +4635,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J157" s="1" t="s">
         <v>480</v>
       </c>
@@ -4640,7 +4646,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J158" s="1" t="s">
         <v>482</v>
       </c>
@@ -4651,7 +4657,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
         <v>483</v>
       </c>
@@ -4677,7 +4683,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J160" s="1" t="s">
         <v>487</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J161" s="1" t="s">
         <v>488</v>
       </c>
@@ -4699,7 +4705,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>33</v>
       </c>
@@ -4707,7 +4713,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>277</v>
       </c>
@@ -4718,7 +4724,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>492</v>
       </c>
@@ -4741,7 +4747,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C165" s="1" t="s">
         <v>496</v>
       </c>
@@ -4767,7 +4773,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J166" s="1" t="s">
         <v>499</v>
       </c>
@@ -4778,7 +4784,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
         <v>500</v>
       </c>
@@ -4804,7 +4810,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J168" s="1" t="s">
         <v>503</v>
       </c>
@@ -4815,7 +4821,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
         <v>504</v>
       </c>
@@ -4832,7 +4838,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C170" s="1" t="s">
         <v>505</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J171" s="1" t="s">
         <v>509</v>
       </c>
@@ -4866,7 +4872,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C172" s="1" t="s">
         <v>510</v>
       </c>
@@ -4892,7 +4898,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C173" s="1" t="s">
         <v>515</v>
       </c>
@@ -4918,7 +4924,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C174" s="1" t="s">
         <v>518</v>
       </c>
@@ -4932,7 +4938,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C175" s="1" t="s">
         <v>519</v>
       </c>
@@ -4958,7 +4964,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C176" s="1" t="s">
         <v>523</v>
       </c>
@@ -4984,7 +4990,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="177" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J177" s="1" t="s">
         <v>527</v>
       </c>
@@ -4995,7 +5001,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="178" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C178" s="1" t="s">
         <v>528</v>
       </c>
@@ -5021,7 +5027,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="179" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J179" s="1" t="s">
         <v>531</v>
       </c>
@@ -5032,7 +5038,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="180" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C180" s="1" t="s">
         <v>532</v>
       </c>
@@ -5061,7 +5067,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="181" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J181" s="1" t="s">
         <v>539</v>
       </c>
@@ -5072,825 +5078,825 @@
         <v>540</v>
       </c>
     </row>
-    <row r="182" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="183" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="184" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="185" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="186" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="187" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="188" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="189" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="190" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="191" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="192" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
fixed textafter method for ellipsis character
</commit_message>
<xml_diff>
--- a/Schablonen/Radiolearn.xlsx
+++ b/Schablonen/Radiolearn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35FED3B-AB91-4F9A-98C8-0A5FDD934BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D0E90A-7C60-4ED8-863F-127A59CFF8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2190" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1955,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G106" workbookViewId="0">
-      <selection activeCell="M126" sqref="M126"/>
+    <sheetView tabSelected="1" topLeftCell="G100" workbookViewId="0">
+      <selection activeCell="K126" sqref="K126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Radiolearn Schablone in Excel und assets
</commit_message>
<xml_diff>
--- a/Schablonen/Radiolearn.xlsx
+++ b/Schablonen/Radiolearn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6E4066-E0EA-4072-8C09-E53156DA31EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8E088D-F02A-4FEA-B589-6845ED299DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2190" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="75" windowWidth="37470" windowHeight="18015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="546">
   <si>
     <t>Gliederung</t>
   </si>
@@ -1126,12 +1126,6 @@
     <t>Pn2</t>
   </si>
   <si>
-    <t>OL / UL / ML</t>
-  </si>
-  <si>
-    <t>OL;Oberfeld;Oberlappen/UL;Unterfeld;Unterlappen/ML;Mittelfeld;Mittellappen</t>
-  </si>
-  <si>
     <t>Pn3</t>
   </si>
   <si>
@@ -1633,9 +1627,6 @@
     <t>... Dislokation</t>
   </si>
   <si>
-    <t>Fraktur [von %S6% ][%S7% Dislokation.]</t>
-  </si>
-  <si>
     <t>Fraktur [von %S6%] [%S7% Dislokation.]</t>
   </si>
   <si>
@@ -1658,6 +1649,15 @@
   </si>
   <si>
     <t>Ausdehnung über … cm</t>
+  </si>
+  <si>
+    <t>frisch / alt</t>
+  </si>
+  <si>
+    <t>frisch/alt</t>
+  </si>
+  <si>
+    <t>Fraktur[ %S8%][ von %S6%][ %S7% Dislokation].</t>
   </si>
 </sst>
 </file>
@@ -1955,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K126" sqref="K126"/>
+    <sheetView tabSelected="1" topLeftCell="H163" workbookViewId="0">
+      <selection activeCell="N180" sqref="N180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3697,7 +3697,7 @@
         <v>316</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="N98" s="1" t="s">
         <v>317</v>
@@ -3976,52 +3976,52 @@
         <v>367</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>368</v>
+        <v>422</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>369</v>
+        <v>423</v>
       </c>
     </row>
     <row r="114" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J114" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="L114" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="K114" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="L114" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="115" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C115" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="N115" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="O115" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="N115" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="O115" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="116" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C116" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J116" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="J116" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="K116" s="2" t="s">
         <v>187</v>
@@ -4030,15 +4030,15 @@
         <v>188</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="O116" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="117" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J117" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>43</v>
@@ -4049,74 +4049,74 @@
     </row>
     <row r="118" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J118" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="M118" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="K118" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="M118" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="119" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J119" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>106</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="120" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J120" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="121" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J121" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M121" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="122" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C122" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="N122" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="N122" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="123" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C123" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K123" s="2" t="s">
         <v>187</v>
@@ -4125,12 +4125,12 @@
         <v>188</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="124" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J124" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>43</v>
@@ -4141,57 +4141,57 @@
     </row>
     <row r="125" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J125" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="L125" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="K125" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="L125" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="126" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J126" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>106</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="127" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J127" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="128" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C129" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="J129" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="J129" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="K129" s="2" t="s">
         <v>187</v>
@@ -4200,26 +4200,26 @@
         <v>188</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="O129" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="130" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J130" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L130" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="K130" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="L130" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="131" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J131" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="K131" s="1" t="s">
         <v>43</v>
@@ -4230,24 +4230,24 @@
     </row>
     <row r="132" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J132" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L132" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="133" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C133" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K133" s="2" t="s">
         <v>187</v>
@@ -4256,15 +4256,15 @@
         <v>188</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="O133" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J134" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>43</v>
@@ -4275,24 +4275,24 @@
     </row>
     <row r="135" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J135" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="L135" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="K135" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="L135" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="136" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C136" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="J136" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="J136" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="K136" s="2" t="s">
         <v>187</v>
@@ -4301,15 +4301,15 @@
         <v>188</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="O136" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="137" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J137" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K137" s="1" t="s">
         <v>43</v>
@@ -4320,24 +4320,24 @@
     </row>
     <row r="138" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J138" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="L138" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="139" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C139" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="K139" s="2" t="s">
         <v>187</v>
@@ -4346,15 +4346,15 @@
         <v>188</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="O139" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J140" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K140" s="1" t="s">
         <v>43</v>
@@ -4365,24 +4365,24 @@
     </row>
     <row r="141" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J141" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="L141" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C142" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="143" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4390,18 +4390,18 @@
         <v>33</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="144" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>16</v>
@@ -4410,21 +4410,21 @@
         <v>38</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="145" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C145" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K145" s="1" t="s">
         <v>43</v>
@@ -4433,94 +4433,94 @@
         <v>213</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="146" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C146" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="147" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C147" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="148" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C148" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="149" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C149" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="150" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C150" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>4</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="151" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C151" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K151" s="1" t="s">
         <v>43</v>
@@ -4529,10 +4529,10 @@
         <v>213</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="152" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4540,18 +4540,18 @@
         <v>33</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="153" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>468</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>16</v>
@@ -4560,21 +4560,21 @@
         <v>38</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="154" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C154" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>43</v>
@@ -4583,44 +4583,44 @@
         <v>213</v>
       </c>
       <c r="N154" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="155" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C155" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N155" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="I155" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="J155" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="K155" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="M155" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="N155" s="1" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="156" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C156" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="J156" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="I156" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="J156" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>43</v>
@@ -4629,18 +4629,18 @@
         <v>213</v>
       </c>
       <c r="N156" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="157" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J157" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>227</v>
@@ -4648,7 +4648,7 @@
     </row>
     <row r="158" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J158" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="K158" s="1" t="s">
         <v>187</v>
@@ -4659,16 +4659,16 @@
     </row>
     <row r="159" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="I159" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="J159" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="I159" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="J159" s="1" t="s">
-        <v>485</v>
       </c>
       <c r="K159" s="1" t="s">
         <v>43</v>
@@ -4677,18 +4677,18 @@
         <v>213</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="160" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J160" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>227</v>
@@ -4696,7 +4696,7 @@
     </row>
     <row r="161" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J161" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="K161" s="1" t="s">
         <v>187</v>
@@ -4710,7 +4710,7 @@
         <v>33</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="163" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4718,24 +4718,24 @@
         <v>277</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="N163" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="164" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>16</v>
@@ -4744,175 +4744,175 @@
         <v>38</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="165" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C165" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J165" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="K165" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L165" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N165" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="166" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J166" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K166" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M166" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="167" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C167" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K167" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L167" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N167" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="168" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J168" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="K168" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="169" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C169" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="N169" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="170" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C170" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="K170" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="L170" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I170" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="J170" s="1" t="s">
+      <c r="N170" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="K170" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="L170" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="N170" s="1" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="171" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J171" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K171" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M171" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="172" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C172" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="K172" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="D172" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="H172" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="I172" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="J172" s="1" t="s">
+      <c r="L172" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="K172" s="1" t="s">
+      <c r="N172" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="L172" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="N172" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="173" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C173" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J173" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K173" s="1" t="s">
         <v>43</v>
@@ -4921,64 +4921,64 @@
         <v>213</v>
       </c>
       <c r="N173" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="174" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C174" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="175" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C175" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="J175" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="D175" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="H175" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="I175" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="J175" s="1" t="s">
-        <v>521</v>
-      </c>
       <c r="K175" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L175" s="1" t="s">
         <v>227</v>
       </c>
       <c r="N175" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="176" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C176" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="J176" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="H176" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="I176" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="J176" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="K176" s="1" t="s">
         <v>43</v>
@@ -4987,15 +4987,15 @@
         <v>213</v>
       </c>
       <c r="N176" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="177" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J177" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K177" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L177" s="1" t="s">
         <v>227</v>
@@ -5003,19 +5003,19 @@
     </row>
     <row r="178" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C178" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H178" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K178" s="1" t="s">
         <v>43</v>
@@ -5024,15 +5024,15 @@
         <v>213</v>
       </c>
       <c r="N178" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="179" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J179" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K179" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L179" s="1" t="s">
         <v>227</v>
@@ -5040,45 +5040,55 @@
     </row>
     <row r="180" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C180" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="J180" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="K180" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="D180" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="I180" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="J180" s="1" t="s">
+      <c r="L180" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="K180" s="1" t="s">
+      <c r="M180" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="L180" s="1" t="s">
+      <c r="N180" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="O180" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="M180" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="N180" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="O180" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="181" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J181" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="K181" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M181" s="1" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="182" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>537</v>
+      </c>
+    </row>
+    <row r="182" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J182" t="s">
+        <v>495</v>
+      </c>
+      <c r="K182" t="s">
+        <v>543</v>
+      </c>
+      <c r="L182" t="s">
+        <v>544</v>
+      </c>
+    </row>
     <row r="183" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="184" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="185" spans="3:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
removed variable ratio in all instances
</commit_message>
<xml_diff>
--- a/Schablonen/Radiolearn.xlsx
+++ b/Schablonen/Radiolearn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F17071-4207-4DCC-8372-CB5403E27CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0540958-D735-4899-BFC1-80F4C475BDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1976,7 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K113" sqref="K113"/>
     </sheetView>
   </sheetViews>

</xml_diff>